<commit_message>
... and all the files I missed
</commit_message>
<xml_diff>
--- a/Domino LED/BOM/Domino LED BOM.xlsx
+++ b/Domino LED/BOM/Domino LED BOM.xlsx
@@ -8,24 +8,25 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino JTAG Rev. A" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino LED Rev. B" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -289,19 +290,19 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2:H10"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.83921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.2470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1686274509804"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.2470588235294"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.9725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.321568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3725490196078"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.356862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.278431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6549019607843"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Domino LED Rev. C: changed Logos
</commit_message>
<xml_diff>
--- a/Domino LED/BOM/Domino LED BOM.xlsx
+++ b/Domino LED/BOM/Domino LED BOM.xlsx
@@ -8,25 +8,26 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino LED Rev. B" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino LED Rev. C" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -294,15 +295,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.321568627451"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3725490196078"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.356862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.278431372549"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4980392156863"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.3647058823529"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4745098039216"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.4980392156863"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.5960784313726"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.86274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Domino LED Rev. D: changed silkscreen font ratio to 20%
</commit_message>
<xml_diff>
--- a/Domino LED/BOM/Domino LED BOM.xlsx
+++ b/Domino LED/BOM/Domino LED BOM.xlsx
@@ -8,26 +8,27 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino LED Rev. C" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino LED Rev. D" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino LED Rev. D'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -295,15 +296,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.88235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4980392156863"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.3647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.4980392156863"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.5960784313726"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.90980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.6352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5058823529412"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.6274509803922"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.6352941176471"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.9137254901961"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.90980392156863"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>